<commit_message>
Update PPT & PDF
</commit_message>
<xml_diff>
--- a/【存储稳定性测试与数据一致性校验】测试用例.xlsx
+++ b/【存储稳定性测试与数据一致性校验】测试用例.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13160" tabRatio="460"/>
+    <workbookView windowWidth="27660" windowHeight="13140" tabRatio="460"/>
   </bookViews>
   <sheets>
     <sheet name="LBA工具测试用例" sheetId="6" r:id="rId1"/>
@@ -2864,14 +2864,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">chaosArsenal故障注入工具: </t>
     </r>
     <r>
@@ -2894,6 +2886,27 @@
         <scheme val="minor"/>
       </rPr>
       <t>https://gitee.com/openeuler/chaosArsenal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF3232F0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF3232F0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://gitee.com/sanjingzi</t>
     </r>
   </si>
   <si>
@@ -7840,20 +7853,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF00B0F0"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="9"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -7867,9 +7867,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF3232F0"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -9824,13 +9837,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
-<customStorage xmlns="https://web.wps.cn/et/2018/main">
-  <book/>
-  <sheets/>
-</customStorage>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -10014,7 +10020,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="25262840" y="24585930"/>
-          <a:ext cx="8730615" cy="6417310"/>
+          <a:ext cx="8730615" cy="6531610"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10278,8 +10284,8 @@
   <sheetPr/>
   <dimension ref="A1:Q138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G110" workbookViewId="0">
-      <selection activeCell="K131" sqref="K131"/>
+    <sheetView tabSelected="1" topLeftCell="K4" workbookViewId="0">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -13392,7 +13398,7 @@
       </c>
       <c r="L118" s="40"/>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" ht="18.3" spans="1:12">
       <c r="A119" s="90"/>
       <c r="B119" s="11"/>
       <c r="C119" s="76" t="s">
@@ -13418,7 +13424,7 @@
       </c>
       <c r="L119" s="40"/>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" ht="18.3" spans="1:12">
       <c r="A120" s="90"/>
       <c r="B120" s="11"/>
       <c r="C120" s="76"/>
@@ -13516,7 +13522,7 @@
       </c>
       <c r="L123" s="40"/>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" ht="18.3" spans="1:12">
       <c r="A124" s="90"/>
       <c r="B124" s="11" t="s">
         <v>454</v>
@@ -13544,7 +13550,7 @@
       </c>
       <c r="L124" s="40"/>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" ht="18.3" spans="1:12">
       <c r="A125" s="90"/>
       <c r="B125" s="11"/>
       <c r="C125" s="76"/>
@@ -13568,7 +13574,7 @@
       </c>
       <c r="L125" s="40"/>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" ht="18.3" spans="1:12">
       <c r="A126" s="90"/>
       <c r="B126" s="11"/>
       <c r="C126" s="91" t="s">
@@ -13594,7 +13600,7 @@
       </c>
       <c r="L126" s="40"/>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" ht="18.3" spans="1:12">
       <c r="A127" s="90"/>
       <c r="B127" s="11"/>
       <c r="C127" s="76"/>

</xml_diff>